<commit_message>
Non-specified (energy) --> Non-specified.
</commit_message>
<xml_diff>
--- a/data-raw/FixedCOLWRLDElect.xlsx
+++ b/data-raw/FixedCOLWRLDElect.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10B03CE-FA9A-3447-B6BE-7194414E1B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18198E2A-FE8F-2D4A-AB14-04BB3B059A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14420" yWindow="500" windowWidth="36780" windowHeight="28300" activeTab="3" xr2:uid="{00C87A90-6B15-DF45-AB5F-3D787AE55E6B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{00C87A90-6B15-DF45-AB5F-3D787AE55E6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="2" r:id="rId1"/>
@@ -26,9 +26,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -465,9 +468,6 @@
     <t>Pumped storage plants</t>
   </si>
   <si>
-    <t>Non-specified (energy)</t>
-  </si>
-  <si>
     <t>Losses</t>
   </si>
   <si>
@@ -553,6 +553,9 @@
   </si>
   <si>
     <t>WRLD</t>
+  </si>
+  <si>
+    <t>Non-specified</t>
   </si>
 </sst>
 </file>
@@ -10934,7 +10937,7 @@
   <dimension ref="A1:AO80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20809,7 +20812,7 @@
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20969,7 +20972,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -20984,7 +20987,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>35</v>
@@ -21019,7 +21022,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -21034,7 +21037,7 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>36</v>
@@ -21069,7 +21072,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -21084,7 +21087,7 @@
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G6" t="s">
         <v>104</v>
@@ -21119,7 +21122,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -21169,7 +21172,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -21219,7 +21222,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -21269,7 +21272,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -21319,7 +21322,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -21334,7 +21337,7 @@
         <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>107</v>
@@ -21369,7 +21372,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
@@ -21384,7 +21387,7 @@
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>108</v>
@@ -21419,7 +21422,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
@@ -21434,7 +21437,7 @@
         <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>109</v>
@@ -21469,7 +21472,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
@@ -21484,7 +21487,7 @@
         <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>110</v>
@@ -21519,7 +21522,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
@@ -21534,7 +21537,7 @@
         <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>111</v>
@@ -21569,7 +21572,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
@@ -21584,7 +21587,7 @@
         <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>112</v>
@@ -21619,7 +21622,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -21634,7 +21637,7 @@
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>113</v>
@@ -21669,7 +21672,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -21684,7 +21687,7 @@
         <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>114</v>
@@ -21719,7 +21722,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -21734,7 +21737,7 @@
         <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>115</v>
@@ -21769,7 +21772,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -21784,7 +21787,7 @@
         <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>116</v>
@@ -21819,7 +21822,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -21834,10 +21837,10 @@
         <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>0</v>
@@ -21869,7 +21872,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
@@ -21884,10 +21887,10 @@
         <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H22" t="s">
         <v>0</v>
@@ -21919,7 +21922,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -21931,13 +21934,13 @@
         <v>17</v>
       </c>
       <c r="E23" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" t="s">
         <v>142</v>
       </c>
-      <c r="F23" t="s">
-        <v>143</v>
-      </c>
       <c r="G23" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>0</v>
@@ -21969,7 +21972,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
@@ -21981,13 +21984,13 @@
         <v>17</v>
       </c>
       <c r="E24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" t="s">
         <v>142</v>
       </c>
-      <c r="F24" t="s">
-        <v>143</v>
-      </c>
       <c r="G24" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>0</v>
@@ -22019,7 +22022,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
@@ -22031,13 +22034,13 @@
         <v>17</v>
       </c>
       <c r="E25" t="s">
+        <v>141</v>
+      </c>
+      <c r="F25" t="s">
         <v>142</v>
       </c>
-      <c r="F25" t="s">
-        <v>143</v>
-      </c>
       <c r="G25" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>0</v>
@@ -22069,7 +22072,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B26" t="s">
         <v>19</v>
@@ -22081,13 +22084,13 @@
         <v>17</v>
       </c>
       <c r="E26" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" t="s">
         <v>142</v>
       </c>
-      <c r="F26" t="s">
-        <v>143</v>
-      </c>
       <c r="G26" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>0</v>
@@ -22119,7 +22122,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B27" t="s">
         <v>19</v>
@@ -22131,13 +22134,13 @@
         <v>17</v>
       </c>
       <c r="E27" t="s">
+        <v>141</v>
+      </c>
+      <c r="F27" t="s">
         <v>142</v>
       </c>
-      <c r="F27" t="s">
-        <v>143</v>
-      </c>
       <c r="G27" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>0</v>
@@ -22169,7 +22172,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B28" t="s">
         <v>19</v>
@@ -22181,13 +22184,13 @@
         <v>17</v>
       </c>
       <c r="E28" t="s">
+        <v>141</v>
+      </c>
+      <c r="F28" t="s">
         <v>142</v>
       </c>
-      <c r="F28" t="s">
-        <v>143</v>
-      </c>
       <c r="G28" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>0</v>
@@ -22219,7 +22222,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B29" t="s">
         <v>19</v>
@@ -22231,13 +22234,13 @@
         <v>17</v>
       </c>
       <c r="E29" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" t="s">
         <v>142</v>
       </c>
-      <c r="F29" t="s">
-        <v>143</v>
-      </c>
       <c r="G29" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>0</v>
@@ -22269,7 +22272,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s">
         <v>19</v>
@@ -22281,13 +22284,13 @@
         <v>17</v>
       </c>
       <c r="E30" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" t="s">
         <v>142</v>
       </c>
-      <c r="F30" t="s">
-        <v>143</v>
-      </c>
       <c r="G30" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>0</v>
@@ -22319,7 +22322,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B31" t="s">
         <v>19</v>
@@ -22331,13 +22334,13 @@
         <v>17</v>
       </c>
       <c r="E31" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" t="s">
         <v>142</v>
       </c>
-      <c r="F31" t="s">
-        <v>143</v>
-      </c>
       <c r="G31" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>0</v>
@@ -22369,7 +22372,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B32" t="s">
         <v>19</v>
@@ -22381,13 +22384,13 @@
         <v>17</v>
       </c>
       <c r="E32" t="s">
+        <v>141</v>
+      </c>
+      <c r="F32" t="s">
         <v>142</v>
       </c>
-      <c r="F32" t="s">
-        <v>143</v>
-      </c>
       <c r="G32" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>0</v>
@@ -22419,7 +22422,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
         <v>19</v>
@@ -22431,13 +22434,13 @@
         <v>17</v>
       </c>
       <c r="E33" t="s">
+        <v>141</v>
+      </c>
+      <c r="F33" t="s">
         <v>142</v>
       </c>
-      <c r="F33" t="s">
-        <v>143</v>
-      </c>
       <c r="G33" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>0</v>
@@ -22469,7 +22472,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B34" t="s">
         <v>19</v>
@@ -22481,13 +22484,13 @@
         <v>17</v>
       </c>
       <c r="E34" t="s">
+        <v>141</v>
+      </c>
+      <c r="F34" t="s">
         <v>142</v>
       </c>
-      <c r="F34" t="s">
-        <v>143</v>
-      </c>
       <c r="G34" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>0</v>
@@ -22519,7 +22522,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
         <v>19</v>
@@ -22531,13 +22534,13 @@
         <v>17</v>
       </c>
       <c r="E35" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" t="s">
         <v>142</v>
       </c>
-      <c r="F35" t="s">
-        <v>143</v>
-      </c>
       <c r="G35" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>0</v>
@@ -22569,7 +22572,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B36" t="s">
         <v>19</v>
@@ -22581,13 +22584,13 @@
         <v>17</v>
       </c>
       <c r="E36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>0</v>
@@ -22619,7 +22622,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
         <v>19</v>
@@ -22631,13 +22634,13 @@
         <v>17</v>
       </c>
       <c r="E37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>0</v>
@@ -22669,7 +22672,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
         <v>19</v>
@@ -22681,13 +22684,13 @@
         <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>0</v>
@@ -22719,7 +22722,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
@@ -22731,13 +22734,13 @@
         <v>17</v>
       </c>
       <c r="E39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>0</v>
@@ -22769,7 +22772,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B40" t="s">
         <v>19</v>
@@ -22781,13 +22784,13 @@
         <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>0</v>
@@ -22819,7 +22822,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
         <v>19</v>
@@ -22831,13 +22834,13 @@
         <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>0</v>
@@ -22869,7 +22872,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
         <v>19</v>
@@ -22881,13 +22884,13 @@
         <v>17</v>
       </c>
       <c r="E42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>0</v>

</xml_diff>